<commit_message>
Added testcases for exp2
</commit_message>
<xml_diff>
--- a/test-cases-2015/Testcases for Computer organisation-Responsive.xlsx
+++ b/test-cases-2015/Testcases for Computer organisation-Responsive.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="146">
   <si>
     <t>S.NO</t>
   </si>
@@ -266,13 +266,206 @@
   </si>
   <si>
     <t>The output shown is 2</t>
+  </si>
+  <si>
+    <t>Output for invalid Input</t>
+  </si>
+  <si>
+    <t>To check working for invalid input</t>
+  </si>
+  <si>
+    <t>1.Click add without clicking any row</t>
+  </si>
+  <si>
+    <t>There should be any output</t>
+  </si>
+  <si>
+    <t>There is no output</t>
+  </si>
+  <si>
+    <t>1. Setup the environment required to perform the experiment.                                                                                   - &gt; Install the client side dependencies.                                                                                                                      - &gt; Install browsers.                                                                                                                                                    - &gt; Install different os like windows, Linux ,ubuntu.          2. Open the experiment and click experiment tag in Navbar. -&gt;Click click here link.         -&gt;Click 5-bit</t>
+  </si>
+  <si>
+    <t>Floating Point Numbers Representation</t>
+  </si>
+  <si>
+    <t>8-bit binary representation</t>
+  </si>
+  <si>
+    <t>To check working of 8-bit binary representation</t>
+  </si>
+  <si>
+    <t>1.Input the value of 0.1 in Decimal number field.             2.Input number of exponents as 1.           3.Click submit</t>
+  </si>
+  <si>
+    <t>The 8-bit output should be 0 0 100110</t>
+  </si>
+  <si>
+    <t>The output is 00100110</t>
+  </si>
+  <si>
+    <t>Binary representation of Integral</t>
+  </si>
+  <si>
+    <t>To check the binary Representation of Integral</t>
+  </si>
+  <si>
+    <t>1.Input the value of 1.2 in Decimal number field.             2.Input number of exponents as 2.           3.Click submit</t>
+  </si>
+  <si>
+    <t>The binary representation of the integral is given as 1.</t>
+  </si>
+  <si>
+    <t>The output is 1.</t>
+  </si>
+  <si>
+    <t>Binary representaion of fraction</t>
+  </si>
+  <si>
+    <t>To check the binary representation of the fraction</t>
+  </si>
+  <si>
+    <t>1.Input the value of 2.25 in Decimal number field.             2.Input number of exponents as 2.           3.Click submit</t>
+  </si>
+  <si>
+    <t>The binary representation of the fraction is given as 01</t>
+  </si>
+  <si>
+    <t>The output is 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass </t>
+  </si>
+  <si>
+    <t>Normalized representation of the number</t>
+  </si>
+  <si>
+    <t>To check the normalized representation of the number</t>
+  </si>
+  <si>
+    <t>1.Input the value of 4.75 in Decimal number field.             2.Input number of exponents as 2.           3.Click submit</t>
+  </si>
+  <si>
+    <t>The normalized form of the number 4.75 is given as 1.0011 X 2^(2)</t>
+  </si>
+  <si>
+    <t>the output is 1.0011 X 2^(2)</t>
+  </si>
+  <si>
+    <t>None
+</t>
+  </si>
+  <si>
+    <t>Mantiss and sign</t>
+  </si>
+  <si>
+    <t>To check Mantiss and sign</t>
+  </si>
+  <si>
+    <t>1.Input the value of -3.75 in decimal number field.             2.Input number of exponents as 2.           3.Click submit</t>
+  </si>
+  <si>
+    <t>The mantiss should be 11100 and sign should be 1</t>
+  </si>
+  <si>
+    <t>The output is 11100 and sign is 1</t>
+  </si>
+  <si>
+    <t>Expone and bias</t>
+  </si>
+  <si>
+    <t>To check Expone and bias</t>
+  </si>
+  <si>
+    <t>1.Input the value of 4.25 in decimal number field.             2.Input number of exponents as 3.           3.Click submit</t>
+  </si>
+  <si>
+    <t>The expone for the given number is 5 and the bias is 3</t>
+  </si>
+  <si>
+    <t>The output is 5 and 3</t>
+  </si>
+  <si>
+    <t>Inference</t>
+  </si>
+  <si>
+    <t>To check the Inference</t>
+  </si>
+  <si>
+    <t>1.Input the value of 4.25 in decimal number field.             2.Input number of exponents as 1.           3.Click submit</t>
+  </si>
+  <si>
+    <t>The inference should give an error of exponent overflow</t>
+  </si>
+  <si>
+    <t>The Inference shows the error of exponent overflow</t>
+  </si>
+  <si>
+    <t>Floating point Numbers</t>
+  </si>
+  <si>
+    <t>To check the floating point numbers</t>
+  </si>
+  <si>
+    <t>1. Setup the environment required to perform the experiment.                                                                                   - &gt; Install the client side dependencies.                                                                                                                      - &gt; Install browsers.                                                                                                                                                    - &gt; Install different os like windows, Linux ,ubuntu.          2. Open the experiment and click experiment tag in Navbar. -&gt;Click click here link.              -&gt; Click Floating point numbers</t>
+  </si>
+  <si>
+    <t>1.Input the Decimal Number as 0.50</t>
+  </si>
+  <si>
+    <t>The no-zero normalized form should be rounded to 0.5 ,The abrupt representaion should be rounded to zero.The denormalized should be accurate at 0.5</t>
+  </si>
+  <si>
+    <t>The output shows normalized form and abrupt form rounded at 0.5 and 0 respectively. The denormalized form shows accurate but does not show 0.5 in the table.</t>
+  </si>
+  <si>
+    <t>1.Input the Decimal Number as 0.75</t>
+  </si>
+  <si>
+    <t>The no-zero normalized form should be rounded to 0.75 ,The abrupt representaion should be rounded to zero.The denormalized should be accurate at 0.75</t>
+  </si>
+  <si>
+    <t>The output show no-zero normalized and abrupt as 0.75 and 0 respectively.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None </t>
+  </si>
+  <si>
+    <t>Invalid Input</t>
+  </si>
+  <si>
+    <t>To check output for invalid input</t>
+  </si>
+  <si>
+    <t>1.Input 10        2.Press Submit</t>
+  </si>
+  <si>
+    <t>There should not be any output</t>
+  </si>
+  <si>
+    <t>Alphanumberic input</t>
+  </si>
+  <si>
+    <t>To check output for Alphanumber input</t>
+  </si>
+  <si>
+    <t>1.Input abc        2.Press Submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Setup the environment required to perform the experiment.                                                                                   - &gt; Install the client side dependencies.                                                                                                                      - &gt; Install browsers.                                                                                                                                                    - &gt; Install different os like windows, Linux ,ubuntu.          2. Open the experiment and click experiment tag in Navbar. -&gt;Click click here link.            </t>
+  </si>
+  <si>
+    <t>1.Input the value of  in decimal number field 10.             2.Input number of exponents as 8.           3.Click submit</t>
+  </si>
+  <si>
+    <t>1.Input the value of  in decimal number field 10.             2.Input number of exponents as abc.           3.Click submit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -308,6 +501,7 @@
       <sz val="9.0"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="4">
     <fill>
@@ -348,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -400,6 +594,9 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1128,6 +1325,569 @@
         <v>28</v>
       </c>
     </row>
+    <row r="20">
+      <c r="E20" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="N20" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="M21" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="N21" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="O21" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O23" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="O24" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="N25" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="N26" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O27" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="N28" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O29" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O30" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M31" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="N31" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="O31" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M32" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="N32" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="O32" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M33" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="N33" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="O33" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M34" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="O34" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G1:M1"/>

</xml_diff>